<commit_message>
mise à jour des documentations
Mise à jour de plusieurs documents + ajout
</commit_message>
<xml_diff>
--- a/Documentations/Journal de travail - Fishermen - KGN.xlsx
+++ b/Documentations/Journal de travail - Fishermen - KGN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12300"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Appréciation journaliére'!$C$4:$C$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Journal!$A$6:$H$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Journal!$A$6:$H$112</definedName>
     <definedName name="base">Journal!$A$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="171">
   <si>
     <t>Jour</t>
   </si>
@@ -519,9 +519,6 @@
     <t>La fonctionnalité qui permet de recevoir une amende lorque nous vendons un poisson trop jeûne a été implémenté.</t>
   </si>
   <si>
-    <t>3:45 h</t>
-  </si>
-  <si>
     <t>Rattrapage de test</t>
   </si>
   <si>
@@ -529,6 +526,27 @@
   </si>
   <si>
     <t>1 h</t>
+  </si>
+  <si>
+    <t>J'ai laissé des camarade tester le jeu. Je ne leur ai rien expliqué, exprés, pour voir si le jeu est facilement compréhensible. Ils ont prit quelques secondes à comprendre le jeu de pêche mais sinon ils ont compris facilement. Ils n'ont pas décerné de bug en particulier.</t>
+  </si>
+  <si>
+    <t>2:15 h</t>
+  </si>
+  <si>
+    <t>Test unitaire</t>
+  </si>
+  <si>
+    <t>un test unitaire sur le système de vente de poisson a été ajouté- il test si les poissons osnt légaux ou non.</t>
+  </si>
+  <si>
+    <t>3 h</t>
+  </si>
+  <si>
+    <t>Imprime la documentation</t>
+  </si>
+  <si>
+    <t>Les documents de mon rapport de projet ont été imprimé</t>
   </si>
 </sst>
 </file>
@@ -981,12 +999,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -994,6 +1006,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1478,11 +1496,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Feuille1"/>
-  <dimension ref="A1:H145"/>
+  <sheetPr codeName="Feuille1" filterMode="1"/>
+  <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H108"/>
+    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,26 +1517,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="7" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
@@ -1584,7 +1602,7 @@
       <c r="A7" s="28">
         <v>44683</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="21">
         <v>0.33333333333333331</v>
       </c>
       <c r="C7" s="30">
@@ -1618,7 +1636,7 @@
       <c r="D8" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="41" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="24" t="s">
@@ -1633,7 +1651,7 @@
       <c r="A9" s="28">
         <v>44683</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="21">
         <v>0.375</v>
       </c>
       <c r="C9" s="30">
@@ -1863,7 +1881,7 @@
         <f>C18-B18</f>
         <v>2.430555555555558E-2</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="29" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="24" t="s">
@@ -1937,13 +1955,13 @@
       <c r="D21" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G21" s="25" t="s">
         <v>51</v>
       </c>
       <c r="H21" s="25"/>
@@ -2012,10 +2030,10 @@
       <c r="E24" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="F24" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="27" t="s">
         <v>86</v>
       </c>
       <c r="H24" s="25" t="s">
@@ -2778,13 +2796,13 @@
         <f>C55-B55</f>
         <v>4.8611111111111049E-2</v>
       </c>
-      <c r="E55" s="23" t="s">
+      <c r="E55" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="26" t="s">
+      <c r="F55" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="G55" s="27" t="s">
+      <c r="G55" s="25" t="s">
         <v>117</v>
       </c>
       <c r="H55" s="25"/>
@@ -2803,13 +2821,13 @@
         <f>C56-B56</f>
         <v>1.3888888888888951E-2</v>
       </c>
-      <c r="E56" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" s="26" t="s">
+      <c r="E56" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G56" s="27" t="s">
+      <c r="G56" s="25" t="s">
         <v>86</v>
       </c>
       <c r="H56" s="25"/>
@@ -2828,13 +2846,13 @@
         <f>C57-B57</f>
         <v>6.25E-2</v>
       </c>
-      <c r="E57" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F57" s="26" t="s">
+      <c r="E57" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="G57" s="27" t="s">
+      <c r="G57" s="25" t="s">
         <v>102</v>
       </c>
       <c r="H57" s="25"/>
@@ -2917,7 +2935,7 @@
       <c r="A61" s="28">
         <v>44693</v>
       </c>
-      <c r="B61" s="21">
+      <c r="B61" s="30">
         <v>0.4236111111111111</v>
       </c>
       <c r="C61" s="30">
@@ -2941,7 +2959,7 @@
       <c r="A62" s="28">
         <v>44693</v>
       </c>
-      <c r="B62" s="21">
+      <c r="B62" s="30">
         <v>0.46527777777777773</v>
       </c>
       <c r="C62" s="30">
@@ -2975,7 +2993,7 @@
         <f>C63-B63</f>
         <v>1.041666666666663E-2</v>
       </c>
-      <c r="E63" s="29" t="s">
+      <c r="E63" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F63" s="26" t="s">
@@ -2990,7 +3008,7 @@
       <c r="A64" s="28">
         <v>44693</v>
       </c>
-      <c r="B64" s="30">
+      <c r="B64" s="21">
         <v>0.63888888888888895</v>
       </c>
       <c r="C64" s="30">
@@ -2999,7 +3017,7 @@
       <c r="D64" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E64" s="29" t="s">
+      <c r="E64" s="23" t="s">
         <v>118</v>
       </c>
       <c r="F64" s="26" t="s">
@@ -3014,7 +3032,7 @@
       <c r="A65" s="28">
         <v>44693</v>
       </c>
-      <c r="B65" s="30">
+      <c r="B65" s="21">
         <v>0.68055555555555547</v>
       </c>
       <c r="C65" s="30">
@@ -3024,7 +3042,7 @@
         <f>C65-B65</f>
         <v>2.4305555555555691E-2</v>
       </c>
-      <c r="E65" s="29" t="s">
+      <c r="E65" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F65" s="26" t="s">
@@ -3132,7 +3150,7 @@
       </c>
       <c r="H69" s="25"/>
     </row>
-    <row r="70" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="28">
         <v>44694</v>
       </c>
@@ -3156,7 +3174,7 @@
       </c>
       <c r="H70" s="25"/>
     </row>
-    <row r="71" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="28">
         <v>44694</v>
       </c>
@@ -3181,7 +3199,7 @@
       </c>
       <c r="H71" s="25"/>
     </row>
-    <row r="72" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="28">
         <v>44694</v>
       </c>
@@ -3297,10 +3315,10 @@
       <c r="E76" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F76" s="24" t="s">
+      <c r="F76" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="G76" s="25" t="s">
+      <c r="G76" s="27" t="s">
         <v>133</v>
       </c>
       <c r="H76" s="25"/>
@@ -3321,10 +3339,10 @@
       <c r="E77" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F77" s="24" t="s">
+      <c r="F77" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="G77" s="25" t="s">
+      <c r="G77" s="27" t="s">
         <v>137</v>
       </c>
       <c r="H77" s="25"/>
@@ -3346,10 +3364,10 @@
       <c r="E78" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F78" s="24" t="s">
+      <c r="F78" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="G78" s="25" t="s">
+      <c r="G78" s="27" t="s">
         <v>86</v>
       </c>
       <c r="H78" s="25"/>
@@ -3374,7 +3392,7 @@
       <c r="F79" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="G79" s="27" t="s">
+      <c r="G79" s="25" t="s">
         <v>144</v>
       </c>
       <c r="H79" s="25"/>
@@ -3398,7 +3416,7 @@
       <c r="F80" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="G80" s="27" t="s">
+      <c r="G80" s="25" t="s">
         <v>141</v>
       </c>
       <c r="H80" s="25"/>
@@ -3423,53 +3441,53 @@
       <c r="F81" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G81" s="27" t="s">
+      <c r="G81" s="25" t="s">
         <v>62</v>
       </c>
       <c r="H81" s="25"/>
     </row>
     <row r="82" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="20">
+      <c r="A82" s="28">
         <v>44698</v>
       </c>
-      <c r="B82" s="21">
+      <c r="B82" s="30">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C82" s="21">
+      <c r="C82" s="30">
         <v>0.44791666666666669</v>
       </c>
       <c r="D82" s="22">
         <f>C82-B82</f>
         <v>3.125E-2</v>
       </c>
-      <c r="E82" s="23" t="s">
+      <c r="E82" s="29" t="s">
         <v>8</v>
       </c>
       <c r="F82" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="G82" s="25" t="s">
+      <c r="G82" s="27" t="s">
         <v>143</v>
       </c>
       <c r="H82" s="25"/>
     </row>
     <row r="83" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="20">
+      <c r="A83" s="28">
         <v>44698</v>
       </c>
-      <c r="B83" s="21">
+      <c r="B83" s="30">
         <v>0.43055555555555558</v>
       </c>
-      <c r="C83" s="21">
+      <c r="C83" s="30">
         <v>0.51041666666666663</v>
       </c>
       <c r="D83" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="E83" s="23" t="s">
+      <c r="E83" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F83" s="26" t="s">
+      <c r="F83" s="24" t="s">
         <v>129</v>
       </c>
       <c r="G83" s="27" t="s">
@@ -3477,23 +3495,23 @@
       </c>
       <c r="H83" s="25"/>
     </row>
-    <row r="84" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="20">
+    <row r="84" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="28">
         <v>44698</v>
       </c>
-      <c r="B84" s="21">
+      <c r="B84" s="30">
         <v>0.5625</v>
       </c>
-      <c r="C84" s="21">
+      <c r="C84" s="30">
         <v>0.61111111111111105</v>
       </c>
       <c r="D84" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E84" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F84" s="26" t="s">
+      <c r="E84" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F84" s="24" t="s">
         <v>147</v>
       </c>
       <c r="G84" s="27" t="s">
@@ -3501,7 +3519,7 @@
       </c>
       <c r="H84" s="25"/>
     </row>
-    <row r="85" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="20">
         <v>44698</v>
       </c>
@@ -3518,15 +3536,15 @@
       <c r="E85" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F85" s="26" t="s">
+      <c r="F85" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G85" s="27" t="s">
+      <c r="G85" s="25" t="s">
         <v>62</v>
       </c>
       <c r="H85" s="25"/>
     </row>
-    <row r="86" spans="1:8" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="20">
         <v>44698</v>
       </c>
@@ -3542,10 +3560,10 @@
       <c r="E86" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F86" s="24" t="s">
+      <c r="F86" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="G86" s="25" t="s">
+      <c r="G86" s="27" t="s">
         <v>146</v>
       </c>
       <c r="H86" s="25"/>
@@ -3591,15 +3609,15 @@
       <c r="E88" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F88" s="24" t="s">
+      <c r="F88" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="G88" s="25" t="s">
+      <c r="G88" s="27" t="s">
         <v>47</v>
       </c>
       <c r="H88" s="25"/>
     </row>
-    <row r="89" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="20">
         <v>44700</v>
       </c>
@@ -3664,10 +3682,10 @@
       <c r="E91" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F91" s="26" t="s">
+      <c r="F91" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="G91" s="27" t="s">
+      <c r="G91" s="25" t="s">
         <v>47</v>
       </c>
       <c r="H91" s="25"/>
@@ -3689,10 +3707,10 @@
       <c r="E92" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F92" s="26" t="s">
+      <c r="F92" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G92" s="27" t="s">
+      <c r="G92" s="25" t="s">
         <v>62</v>
       </c>
       <c r="H92" s="25"/>
@@ -3762,15 +3780,15 @@
       <c r="E95" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F95" s="24" t="s">
+      <c r="F95" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="G95" s="25" t="s">
+      <c r="G95" s="27" t="s">
         <v>62</v>
       </c>
       <c r="H95" s="25"/>
     </row>
-    <row r="96" spans="1:8" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="20">
         <v>44701</v>
       </c>
@@ -3794,7 +3812,7 @@
       </c>
       <c r="H96" s="25"/>
     </row>
-    <row r="97" spans="1:8" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="20">
         <v>44701</v>
       </c>
@@ -3843,7 +3861,7 @@
       </c>
       <c r="H98" s="25"/>
     </row>
-    <row r="99" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="20">
         <v>44704</v>
       </c>
@@ -3867,7 +3885,7 @@
       </c>
       <c r="H99" s="25"/>
     </row>
-    <row r="100" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="20">
         <v>44704</v>
       </c>
@@ -3884,15 +3902,15 @@
       <c r="E100" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F100" s="24" t="s">
+      <c r="F100" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="G100" s="25" t="s">
+      <c r="G100" s="27" t="s">
         <v>157</v>
       </c>
       <c r="H100" s="25"/>
     </row>
-    <row r="101" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="20">
         <v>44704</v>
       </c>
@@ -3917,7 +3935,7 @@
       </c>
       <c r="H101" s="25"/>
     </row>
-    <row r="102" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="20">
         <v>44704</v>
       </c>
@@ -3941,7 +3959,7 @@
       </c>
       <c r="H102" s="25"/>
     </row>
-    <row r="103" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="20">
         <v>44704</v>
       </c>
@@ -3958,15 +3976,15 @@
       <c r="E103" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F103" s="26" t="s">
+      <c r="F103" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G103" s="27" t="s">
+      <c r="G103" s="25" t="s">
         <v>86</v>
       </c>
       <c r="H103" s="25"/>
     </row>
-    <row r="104" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="20">
         <v>44705</v>
       </c>
@@ -3974,154 +3992,196 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C104" s="21">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="D104" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E104" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F104" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G104" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H104" s="25"/>
+    </row>
+    <row r="105" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="20">
+        <v>44705</v>
+      </c>
+      <c r="B105" s="21">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C105" s="21">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D104" s="22" t="s">
+      <c r="D105" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="E105" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F105" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="G105" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="H105" s="25"/>
+    </row>
+    <row r="106" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="20">
+        <v>44705</v>
+      </c>
+      <c r="B106" s="21">
+        <v>0.5625</v>
+      </c>
+      <c r="C106" s="21">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D106" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E106" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F106" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="G106" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="H106" s="25"/>
+    </row>
+    <row r="107" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="20">
+        <v>44705</v>
+      </c>
+      <c r="B107" s="21">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C107" s="21">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D107" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E107" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="E104" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F104" s="26" t="s">
+      <c r="G107" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="H107" s="25"/>
+    </row>
+    <row r="108" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="28">
+        <v>44705</v>
+      </c>
+      <c r="B108" s="21">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C108" s="21">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="D108" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="E108" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F108" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="G104" s="27" t="s">
+      <c r="G108" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="H104" s="25"/>
-    </row>
-    <row r="105" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="28">
+      <c r="H108" s="25"/>
+    </row>
+    <row r="109" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="28">
         <v>44705</v>
       </c>
-      <c r="B105" s="21">
+      <c r="B109" s="21">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="C109" s="21">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D109" s="22">
+        <f>C109-B109</f>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="E109" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F109" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G109" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="H109" s="25"/>
+    </row>
+    <row r="110" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="28">
+        <v>44711</v>
+      </c>
+      <c r="B110" s="21">
         <v>0.5625</v>
       </c>
-      <c r="C105" s="21">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="D105" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="E105" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F105" s="24" t="s">
+      <c r="C110" s="21">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D110" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="E110" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F110" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="G105" s="25" t="s">
+      <c r="G110" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H105" s="25"/>
-    </row>
-    <row r="106" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="28">
-        <v>44705</v>
-      </c>
-      <c r="B106" s="21">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="C106" s="21">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="D106" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="E106" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F106" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="G106" s="25" t="s">
+      <c r="H110" s="25"/>
+    </row>
+    <row r="111" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="20">
+        <v>44712</v>
+      </c>
+      <c r="B111" s="21">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C111" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D111" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="H106" s="25"/>
-    </row>
-    <row r="107" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="28">
-        <v>44705</v>
-      </c>
-      <c r="B107" s="21">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="C107" s="21">
-        <v>0.69097222222222221</v>
-      </c>
-      <c r="D107" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="E107" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F107" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="G107" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="H107" s="25"/>
-    </row>
-    <row r="108" spans="1:8" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="20">
-        <v>44705</v>
-      </c>
-      <c r="B108" s="21">
-        <v>0.69097222222222221</v>
-      </c>
-      <c r="C108" s="21">
-        <v>0.70486111111111116</v>
-      </c>
-      <c r="D108" s="22">
-        <f>C108-B108</f>
-        <v>1.3888888888888951E-2</v>
-      </c>
-      <c r="E108" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F108" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="G108" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="H108" s="27"/>
-    </row>
-    <row r="109" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="31"/>
-      <c r="B109" s="11"/>
-      <c r="C109" s="10"/>
-      <c r="D109" s="32"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="13"/>
-      <c r="G109" s="13"/>
-      <c r="H109" s="13"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="10"/>
-      <c r="B110" s="11"/>
-      <c r="C110" s="10"/>
-      <c r="D110" s="12"/>
-      <c r="E110" s="12"/>
-      <c r="F110" s="13"/>
-      <c r="G110" s="13"/>
-      <c r="H110" s="13"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="10"/>
-      <c r="B111" s="11"/>
-      <c r="C111" s="10"/>
-      <c r="D111" s="12"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="13"/>
-      <c r="G111" s="13"/>
-      <c r="H111" s="13"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="10"/>
+      <c r="E111" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F111" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="G111" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="H111" s="27"/>
+    </row>
+    <row r="112" spans="1:8" ht="48" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="31"/>
       <c r="B112" s="11"/>
       <c r="C112" s="10"/>
-      <c r="D112" s="12"/>
+      <c r="D112" s="32"/>
       <c r="E112" s="12"/>
       <c r="F112" s="13"/>
       <c r="G112" s="13"/>
@@ -4457,12 +4517,47 @@
       <c r="G145" s="13"/>
       <c r="H145" s="13"/>
     </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" s="10"/>
+      <c r="B146" s="11"/>
+      <c r="C146" s="10"/>
+      <c r="D146" s="12"/>
+      <c r="E146" s="12"/>
+      <c r="F146" s="13"/>
+      <c r="G146" s="13"/>
+      <c r="H146" s="13"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="10"/>
+      <c r="B147" s="11"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="12"/>
+      <c r="E147" s="12"/>
+      <c r="F147" s="13"/>
+      <c r="G147" s="13"/>
+      <c r="H147" s="13"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" s="10"/>
+      <c r="B148" s="11"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="12"/>
+      <c r="E148" s="12"/>
+      <c r="F148" s="13"/>
+      <c r="G148" s="13"/>
+      <c r="H148" s="13"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <autoFilter ref="A6:H109">
-    <sortState ref="A7:H109">
-      <sortCondition ref="A7:A109"/>
-      <sortCondition ref="B7:B109"/>
+  <autoFilter ref="A6:H112">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <sortState ref="A7:H111">
+      <sortCondition ref="A7:A112"/>
+      <sortCondition ref="B7:B112"/>
     </sortState>
   </autoFilter>
   <sortState ref="A7:H13">
@@ -4510,7 +4605,7 @@
           <x14:formula1>
             <xm:f>Paramètres!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E19:E108 E7:E17</xm:sqref>
+          <xm:sqref>E22:E111 E7:E20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4520,10 +4615,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G18"/>
+  <dimension ref="B1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4536,14 +4631,14 @@
   <sheetData>
     <row r="1" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
     </row>
     <row r="3" spans="2:7" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="37"/>
@@ -4760,6 +4855,34 @@
         <v>71</v>
       </c>
       <c r="F18" s="36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" ht="69" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="33">
+        <v>44711</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" ht="69" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="33">
+        <v>44712</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="36" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4875,12 +4998,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5067,15 +5187,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{958F7502-934F-41DD-8A96-9B5DD575AFBF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F030087-15DC-4EDA-9907-372A451C849E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c00db93e-a012-41a1-8dae-1f2fb8b40d56"/>
+    <ds:schemaRef ds:uri="0119da2b-60ce-4773-88fa-ebab2cde1f55"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5100,18 +5232,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F030087-15DC-4EDA-9907-372A451C849E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{958F7502-934F-41DD-8A96-9B5DD575AFBF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c00db93e-a012-41a1-8dae-1f2fb8b40d56"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0119da2b-60ce-4773-88fa-ebab2cde1f55"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>